<commit_message>
writing to json file
</commit_message>
<xml_diff>
--- a/javascript_test/Json_data_from_truck.xlsx
+++ b/javascript_test/Json_data_from_truck.xlsx
@@ -3,58 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
-  <sheets>
-    <sheet sheetId="1" name="json" state="visible" r:id="rId4"/>
-  </sheets>
   <calcPr calcId="171027"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
-  <si>
-    <t>truckIdSerial</t>
-  </si>
-  <si>
-    <t>canId</t>
-  </si>
-  <si>
-    <t>strCanData</t>
-  </si>
-  <si>
-    <t>systemTickTimestamp</t>
-  </si>
-  <si>
-    <t>dateHourSecondsTimeReceived</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>canId123</t>
-  </si>
-  <si>
-    <t>strCanData123</t>
-  </si>
-  <si>
-    <t>1667218442221</t>
-  </si>
-  <si>
-    <t>31_10_2022_00:14:02.222</t>
-  </si>
-  <si>
-    <t>canId000</t>
-  </si>
-  <si>
-    <t>strCanData000</t>
-  </si>
-  <si>
-    <t>166721844333</t>
-  </si>
-  <si>
-    <t>31_10_2022_00:14:02.333</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -425,66 +375,4 @@
   </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
-</file>
-
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-</worksheet>
 </file>
</xml_diff>